<commit_message>
updates new csv files, sss, philhealth
</commit_message>
<xml_diff>
--- a/src/main/resources/data/philhealth.xlsx
+++ b/src/main/resources/data/philhealth.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="90" windowWidth="20940" windowHeight="10110"/>
@@ -16,34 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
-  <si>
-    <t>Monthly</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Salary Bracket </t>
-  </si>
-  <si>
-    <t>Salary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Range </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Base </t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Premium </t>
-  </si>
-  <si>
-    <t>Employee Share</t>
-  </si>
-  <si>
-    <t>Employer Share</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t xml:space="preserve">4,999.99 and below </t>
   </si>
@@ -124,6 +97,24 @@
   </si>
   <si>
     <t xml:space="preserve">30,000.00 and up </t>
+  </si>
+  <si>
+    <t>Monthly Salary Bracket</t>
+  </si>
+  <si>
+    <t>Monthly Salary Range</t>
+  </si>
+  <si>
+    <t>Salary Base</t>
+  </si>
+  <si>
+    <t>Employer Share (50% of TMC)</t>
+  </si>
+  <si>
+    <t>Employee Share (50% of TMC)</t>
+  </si>
+  <si>
+    <t>Total Monthly Contribution(TMC)</t>
   </si>
 </sst>
 </file>
@@ -159,9 +150,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -463,601 +457,585 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="26.42578125" customWidth="1"/>
     <col min="2" max="2" width="26.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>4000</v>
+      </c>
+      <c r="D2">
+        <v>100</v>
+      </c>
+      <c r="E2">
+        <v>50</v>
+      </c>
+      <c r="F2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>5000</v>
+      </c>
+      <c r="D3">
+        <v>125</v>
+      </c>
+      <c r="E3">
+        <v>62.5</v>
+      </c>
+      <c r="F3">
+        <v>62.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C4" s="1">
+        <v>6000</v>
+      </c>
+      <c r="D4">
+        <v>150</v>
+      </c>
+      <c r="E4">
+        <v>75</v>
+      </c>
+      <c r="F4">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1">
+        <v>7000</v>
+      </c>
+      <c r="D5">
+        <v>175</v>
+      </c>
+      <c r="E5">
+        <v>87.5</v>
+      </c>
+      <c r="F5">
+        <v>87.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="C6" s="1">
+        <v>8000</v>
+      </c>
+      <c r="D6">
+        <v>200</v>
+      </c>
+      <c r="E6">
+        <v>100</v>
+      </c>
+      <c r="F6">
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1">
-        <v>4000</v>
+        <v>9000</v>
       </c>
       <c r="D7">
-        <v>100</v>
+        <v>225</v>
       </c>
       <c r="E7">
-        <v>50</v>
+        <v>112.5</v>
       </c>
       <c r="F7">
-        <v>50</v>
+        <v>112.5</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C8" s="1">
-        <v>5000</v>
+        <v>10000</v>
       </c>
       <c r="D8">
+        <v>250</v>
+      </c>
+      <c r="E8">
         <v>125</v>
       </c>
-      <c r="E8">
-        <v>62.5</v>
-      </c>
       <c r="F8">
-        <v>62.5</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C9" s="1">
-        <v>6000</v>
+        <v>11000</v>
       </c>
       <c r="D9">
-        <v>150</v>
+        <v>275</v>
       </c>
       <c r="E9">
-        <v>75</v>
+        <v>137.5</v>
       </c>
       <c r="F9">
-        <v>75</v>
+        <v>137.5</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C10" s="1">
-        <v>7000</v>
+        <v>12000</v>
       </c>
       <c r="D10">
-        <v>175</v>
+        <v>300</v>
       </c>
       <c r="E10">
-        <v>87.5</v>
+        <v>150</v>
       </c>
       <c r="F10">
-        <v>87.5</v>
+        <v>150</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C11" s="1">
-        <v>8000</v>
+        <v>13000</v>
       </c>
       <c r="D11">
-        <v>200</v>
+        <v>325</v>
       </c>
       <c r="E11">
-        <v>100</v>
+        <v>162.5</v>
       </c>
       <c r="F11">
-        <v>100</v>
+        <v>162.5</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C12" s="1">
-        <v>9000</v>
+        <v>14000</v>
       </c>
       <c r="D12">
-        <v>225</v>
+        <v>350</v>
       </c>
       <c r="E12">
-        <v>112.5</v>
+        <v>175</v>
       </c>
       <c r="F12">
-        <v>112.5</v>
+        <v>175</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C13" s="1">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="D13">
-        <v>250</v>
+        <v>375</v>
       </c>
       <c r="E13">
-        <v>125</v>
+        <v>187.5</v>
       </c>
       <c r="F13">
-        <v>125</v>
+        <v>187.5</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C14" s="1">
-        <v>11000</v>
+        <v>16000</v>
       </c>
       <c r="D14">
-        <v>275</v>
+        <v>400</v>
       </c>
       <c r="E14">
-        <v>137.5</v>
+        <v>200</v>
       </c>
       <c r="F14">
-        <v>137.5</v>
+        <v>200</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C15" s="1">
-        <v>12000</v>
+        <v>17000</v>
       </c>
       <c r="D15">
-        <v>300</v>
+        <v>425</v>
       </c>
       <c r="E15">
-        <v>150</v>
+        <v>212.5</v>
       </c>
       <c r="F15">
-        <v>150</v>
+        <v>212.5</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C16" s="1">
-        <v>13000</v>
+        <v>18000</v>
       </c>
       <c r="D16">
-        <v>325</v>
+        <v>450</v>
       </c>
       <c r="E16">
-        <v>162.5</v>
+        <v>225</v>
       </c>
       <c r="F16">
-        <v>162.5</v>
+        <v>225</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C17" s="1">
-        <v>14000</v>
+        <v>19000</v>
       </c>
       <c r="D17">
-        <v>350</v>
+        <v>475</v>
       </c>
       <c r="E17">
-        <v>175</v>
+        <v>237.5</v>
       </c>
       <c r="F17">
-        <v>175</v>
+        <v>237.5</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C18" s="1">
-        <v>15000</v>
+        <v>20000</v>
       </c>
       <c r="D18">
-        <v>375</v>
+        <v>500</v>
       </c>
       <c r="E18">
-        <v>187.5</v>
+        <v>250</v>
       </c>
       <c r="F18">
-        <v>187.5</v>
+        <v>250</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C19" s="1">
-        <v>16000</v>
+        <v>21000</v>
       </c>
       <c r="D19">
-        <v>400</v>
+        <v>525</v>
       </c>
       <c r="E19">
-        <v>200</v>
+        <v>262.5</v>
       </c>
       <c r="F19">
-        <v>200</v>
+        <v>262.5</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C20" s="1">
-        <v>17000</v>
+        <v>22000</v>
       </c>
       <c r="D20">
-        <v>425</v>
+        <v>550</v>
       </c>
       <c r="E20">
-        <v>212.5</v>
+        <v>275</v>
       </c>
       <c r="F20">
-        <v>212.5</v>
+        <v>275</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C21" s="1">
-        <v>18000</v>
+        <v>23000</v>
       </c>
       <c r="D21">
-        <v>450</v>
+        <v>575</v>
       </c>
       <c r="E21">
-        <v>225</v>
+        <v>287.5</v>
       </c>
       <c r="F21">
-        <v>225</v>
+        <v>287.5</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C22" s="1">
-        <v>19000</v>
+        <v>24000</v>
       </c>
       <c r="D22">
-        <v>475</v>
+        <v>600</v>
       </c>
       <c r="E22">
-        <v>237.5</v>
+        <v>300</v>
       </c>
       <c r="F22">
-        <v>237.5</v>
+        <v>300</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C23" s="1">
-        <v>20000</v>
+        <v>25000</v>
       </c>
       <c r="D23">
-        <v>500</v>
+        <v>625</v>
       </c>
       <c r="E23">
-        <v>250</v>
+        <v>312.5</v>
       </c>
       <c r="F23">
-        <v>250</v>
+        <v>312.5</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C24" s="1">
-        <v>21000</v>
+        <v>26000</v>
       </c>
       <c r="D24">
-        <v>525</v>
+        <v>650</v>
       </c>
       <c r="E24">
-        <v>262.5</v>
+        <v>325</v>
       </c>
       <c r="F24">
-        <v>262.5</v>
+        <v>325</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C25" s="1">
-        <v>22000</v>
+        <v>27000</v>
       </c>
       <c r="D25">
-        <v>550</v>
+        <v>675</v>
       </c>
       <c r="E25">
-        <v>275</v>
+        <v>337.5</v>
       </c>
       <c r="F25">
-        <v>275</v>
+        <v>337.5</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C26" s="1">
-        <v>23000</v>
+        <v>28000</v>
       </c>
       <c r="D26">
-        <v>575</v>
+        <v>700</v>
       </c>
       <c r="E26">
-        <v>287.5</v>
+        <v>350</v>
       </c>
       <c r="F26">
-        <v>287.5</v>
+        <v>350</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C27" s="1">
-        <v>24000</v>
+        <v>29000</v>
       </c>
       <c r="D27">
-        <v>600</v>
+        <v>725</v>
       </c>
       <c r="E27">
-        <v>300</v>
+        <v>362.5</v>
       </c>
       <c r="F27">
-        <v>300</v>
+        <v>362.5</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C28" s="1">
-        <v>25000</v>
+        <v>30000</v>
       </c>
       <c r="D28">
-        <v>625</v>
+        <v>750</v>
       </c>
       <c r="E28">
-        <v>312.5</v>
+        <v>375</v>
       </c>
       <c r="F28">
-        <v>312.5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>23</v>
-      </c>
-      <c r="B29" t="s">
-        <v>31</v>
-      </c>
-      <c r="C29" s="1">
-        <v>26000</v>
-      </c>
-      <c r="D29">
-        <v>650</v>
-      </c>
-      <c r="E29">
-        <v>325</v>
-      </c>
-      <c r="F29">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>24</v>
-      </c>
-      <c r="B30" t="s">
-        <v>32</v>
-      </c>
-      <c r="C30" s="1">
-        <v>27000</v>
-      </c>
-      <c r="D30">
-        <v>675</v>
-      </c>
-      <c r="E30">
-        <v>337.5</v>
-      </c>
-      <c r="F30">
-        <v>337.5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>25</v>
-      </c>
-      <c r="B31" t="s">
-        <v>33</v>
-      </c>
-      <c r="C31" s="1">
-        <v>28000</v>
-      </c>
-      <c r="D31">
-        <v>700</v>
-      </c>
-      <c r="E31">
-        <v>350</v>
-      </c>
-      <c r="F31">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>26</v>
-      </c>
-      <c r="B32" t="s">
-        <v>34</v>
-      </c>
-      <c r="C32" s="1">
-        <v>29000</v>
-      </c>
-      <c r="D32">
-        <v>725</v>
-      </c>
-      <c r="E32">
-        <v>362.5</v>
-      </c>
-      <c r="F32">
-        <v>362.5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>27</v>
-      </c>
-      <c r="B33" t="s">
-        <v>35</v>
-      </c>
-      <c r="C33" s="1">
-        <v>30000</v>
-      </c>
-      <c r="D33">
-        <v>750</v>
-      </c>
-      <c r="E33">
-        <v>375</v>
-      </c>
-      <c r="F33">
         <v>375</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>